<commit_message>
se organizan casos de prueba en gestion de activos corregir CP_GESACT_004 *
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionActivos.xlsx
+++ b/docs/test-cases/gestionActivos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatización v2\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE80CC6-C701-4CC2-90BB-964F5A8AAFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="GestionActivos" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>ID Caso</t>
   </si>
@@ -89,37 +88,15 @@
     <t>CP_GESACT_001</t>
   </si>
   <si>
-    <t>Acceso al módulo Gestión de Activos</t>
-  </si>
-  <si>
     <t>CP_GESACT_002</t>
   </si>
   <si>
-    <t>Seleccionar entidad y elemento secundario</t>
-  </si>
-  <si>
-    <t>1.Abrir modal de filtros
-2.Desplegar select de filtros.
-3.Diligenciar el campo de ID_DEAL
-4.Clic en "Aplicar filtros"</t>
-  </si>
-  <si>
     <t>CP_GESACT_003</t>
   </si>
   <si>
-    <t>Selección de tipo de dispositivo “ONT”</t>
-  </si>
-  <si>
     <t>Caso anterior completado.</t>
   </si>
   <si>
-    <t>7. En la tabla, seleccionar la opción que contenga “ont”.
-8. Clic en Siguiente.</t>
-  </si>
-  <si>
-    <t>Dispositivo ONT disponible</t>
-  </si>
-  <si>
     <t>Texto “elemento secundario” presente</t>
   </si>
   <si>
@@ -129,44 +106,16 @@
     <t>El sistema abre correctamente la aplicación Gestión de Activos.</t>
   </si>
   <si>
-    <t>El sistema permite seleccionar la entidad “elemento secundario” y avanzar al siguiente paso.</t>
-  </si>
-  <si>
-    <t>El sistema permite seleccionar el tipo de dispositivo ONT y continuar el flujo.</t>
-  </si>
-  <si>
     <t>El sistema abrió la aplicación Gestión de Activos según lo esperado.</t>
   </si>
   <si>
-    <t>La entidad “elemento secundario” fue seleccionada y se avanzó al siguiente paso.</t>
-  </si>
-  <si>
-    <t>Se seleccionó el dispositivo ONT y se continuó el flujo correctamente.</t>
-  </si>
-  <si>
     <t>CP_GESACT_004</t>
   </si>
   <si>
-    <t>Selección de dispositivo con estado FAILED</t>
-  </si>
-  <si>
-    <t>9. Seleccionar fila con ID 9 “FAILED”.
-10. Clic en FINALIZAR y esperar que finalice el progreso..</t>
-  </si>
-  <si>
-    <t>Registro con estado FAILED</t>
-  </si>
-  <si>
     <t>El sistema registra la selección y finaliza el proceso mostrando la barra de progreso y completando la acción.</t>
   </si>
   <si>
     <t>Se seleccionó el registro con estado FAILED y la finalización se ejecutó correctamente.</t>
-  </si>
-  <si>
-    <t>CP_GESACT_005</t>
-  </si>
-  <si>
-    <t>Actualización de estado operativo a LOST</t>
   </si>
   <si>
     <t>11. Seleccionar primer registro de la tabla (capturar FACTORYSERIAL).
@@ -186,12 +135,6 @@
     <t>El estado operativo fue actualizado a LOST y el modal se cerró correctamente.</t>
   </si>
   <si>
-    <t>CP_GESACT_006</t>
-  </si>
-  <si>
-    <t>Repetición de flujo de selección de entidad y dispositivo para registro con estado LOST</t>
-  </si>
-  <si>
     <t>Haber actualizado el estado en el caso anterior.</t>
   </si>
   <si>
@@ -207,35 +150,31 @@
     <t>El flujo se completó correctamente para el registro con estado LOST.</t>
   </si>
   <si>
-    <t>CP_GESACT_007</t>
-  </si>
-  <si>
-    <t>Filtrado de registros por FACTORYSERIAL capturado</t>
-  </si>
-  <si>
-    <t>Haber capturado el FACTORYSERIAL en el paso 11.</t>
-  </si>
-  <si>
-    <t>24. Clic en Mostrar filtro.
-25. Abrir selector de campo y escoger FACTORYSERIAL.
-26. Diligenciar el serial capturado.
-27. Clic en Aplicar filtro y esperar a que finalice el progreso.</t>
-  </si>
-  <si>
-    <t>FACTORYSERIAL capturado previamente</t>
-  </si>
-  <si>
-    <t>La tabla de resultados se filtra mostrando únicamente el registro que coincide con el FACTORYSERIAL ingresado.</t>
-  </si>
-  <si>
-    <t>La tabla se filtró correctamente mostrando solo el registro con el FACTORYSERIAL indicado.</t>
+    <t>Acceso al la vista Gestión de Activos</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Seleccionar entidad"
+2.Clic en botón "Siguiente"
+3.Seleccionar "ont"
+4.Clic en botón "Siguiente"
+5.Seleccionar fila con ID 9 "FAILED"
+6.Hacer clic en el botón "FINALIZAR"</t>
+  </si>
+  <si>
+    <t>Filtrar ont por estado en "FAILED"</t>
+  </si>
+  <si>
+    <t>actualizacion de estado de la ont FAILED a LOST</t>
+  </si>
+  <si>
+    <t>Validar actualización de ont a estado LOST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,14 +601,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
@@ -685,7 +624,7 @@
     <col min="12" max="12" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,12 +662,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="98.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -743,13 +682,13 @@
         <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>16</v>
@@ -762,12 +701,12 @@
       </c>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="148.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -779,16 +718,16 @@
         <v>14</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>16</v>
@@ -801,12 +740,12 @@
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="171" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -815,19 +754,19 @@
         <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>16</v>
@@ -840,12 +779,12 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="171" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -854,19 +793,19 @@
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>16</v>
@@ -878,125 +817,9 @@
         <v>18</v>
       </c>
       <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se unifica el caso de prueba CP_GESACT_003 en gestion activos
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionActivos.xlsx
+++ b/docs/test-cases/gestionActivos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>ID Caso</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>El sistema abrió la aplicación Gestión de Activos según lo esperado.</t>
-  </si>
-  <si>
-    <t>CP_GESACT_004</t>
   </si>
   <si>
     <t>El sistema registra la selección y finaliza el proceso mostrando la barra de progreso y completando la acción.</t>
@@ -135,21 +132,6 @@
     <t>El estado operativo fue actualizado a LOST y el modal se cerró correctamente.</t>
   </si>
   <si>
-    <t>Haber actualizado el estado en el caso anterior.</t>
-  </si>
-  <si>
-    <t>17–23. Repetir selección de entidad “elemento secundario”, tipo “ONT”, seleccionar fila con ID 10 “LOST”, clic en FINALIZAR y esperar la barra de progreso.</t>
-  </si>
-  <si>
-    <t>Registro con estado LOST</t>
-  </si>
-  <si>
-    <t>El sistema completa nuevamente el flujo para el dispositivo con estado LOST.</t>
-  </si>
-  <si>
-    <t>El flujo se completó correctamente para el registro con estado LOST.</t>
-  </si>
-  <si>
     <t>Acceso al la vista Gestión de Activos</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
   </si>
   <si>
     <t>actualizacion de estado de la ont FAILED a LOST</t>
-  </si>
-  <si>
-    <t>Validar actualización de ont a estado LOST</t>
   </si>
 </sst>
 </file>
@@ -602,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -667,7 +646,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -706,7 +685,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -718,16 +697,16 @@
         <v>14</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>16</v>
@@ -745,7 +724,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -757,16 +736,16 @@
         <v>22</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>16</v>
@@ -778,45 +757,6 @@
         <v>18</v>
       </c>
       <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:13" ht="171" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se realizan cambios en la enumeracion en gestion de activos y se organiza caso de prueba en el documento
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionActivos.xlsx
+++ b/docs/test-cases/gestionActivos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatización v2\Automatizacion\docs\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB26887-14B4-4155-8FAD-46C69D7DF1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GestionActivos" sheetId="1" r:id="rId1"/>
@@ -115,21 +116,7 @@
     <t>Se seleccionó el registro con estado FAILED y la finalización se ejecutó correctamente.</t>
   </si>
   <si>
-    <t>11. Seleccionar primer registro de la tabla (capturar FACTORYSERIAL).
-12. Clic en Actualizar estado operativo.
-13. Abrir lista de estados.
-14. Seleccionar LOST.
-15. Diligenciar comentario “test automatización”.
-16. Clic en Guardar.</t>
-  </si>
-  <si>
     <t>Serial ONT válido</t>
-  </si>
-  <si>
-    <t>El estado operativo del dispositivo se actualiza a LOST y se cierra el modal.</t>
-  </si>
-  <si>
-    <t>El estado operativo fue actualizado a LOST y el modal se cerró correctamente.</t>
   </si>
   <si>
     <t>Acceso al la vista Gestión de Activos</t>
@@ -146,14 +133,40 @@
     <t>Filtrar ont por estado en "FAILED"</t>
   </si>
   <si>
-    <t>actualizacion de estado de la ont FAILED a LOST</t>
+    <t>1.Seleccionar el primer registro de la tabla
+2.Clic en el botón "Actualizar estado operativo"
+3.Clic en estado para mostrar la lista opciones.
+4.Seleccionar la opción "LOST" en el estado
+5.Diligenciar el campo de comentario con "test automatización"
+6.Clic en botón "Guardar" para actualizar estado ont
+7.Clic en botón "Seleccionar entidad"
+8.Seleccionar la fila que contiene el texto "elemento secundario"
+9.Clic en botón "Siguiente"
+10.Seleccionar "ont"
+11.Clic en botón "Siguiente"
+12.Seleccionar fila con ID 10 "LOST"
+13.Hacer clic en el botón "FINALIZAR"
+14.Clic en el botón "Mostrar filtro"
+15.Clic en el estado para mostrar la lista de opciones.
+16.Seleccionar opción "FACTORYSERIAL" en la lista de opciones
+17.Diligenciar campo de texto con serial ONT capturado previamente
+18.Clic en botón "Aplicar filtro"</t>
+  </si>
+  <si>
+    <t>El estado FAILED del dispositivo se actualiza a LOST y se cierra el modal.</t>
+  </si>
+  <si>
+    <t>La tabla se filtró correctamente mostrando solo el registro con el FACTORYSERIAL indicado.</t>
+  </si>
+  <si>
+    <t>Actualiza ONT a LOST y valida filtrado por FACTORYSERIAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,14 +593,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
@@ -603,7 +616,7 @@
     <col min="12" max="12" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,12 +654,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="98.25" customHeight="1">
+    <row r="2" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -680,12 +693,12 @@
       </c>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="148.5" customHeight="1">
+    <row r="3" spans="1:13" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -697,7 +710,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>23</v>
@@ -719,7 +732,7 @@
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="171" customHeight="1">
+    <row r="4" spans="1:13" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -736,16 +749,16 @@
         <v>22</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
se modifica diagramas y archivos de excel, corregir diagrama contenido clases de negocio
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionActivos.xlsx
+++ b/docs/test-cases/gestionActivos.xlsx
@@ -112,14 +112,6 @@
     <t>Acceso al la vista Gestión de Activos</t>
   </si>
   <si>
-    <t>1.Clic en botón "Seleccionar entidad"
-2.Clic en botón "Siguiente"
-3.Seleccionar "ont"
-4.Clic en botón "Siguiente"
-5.Seleccionar fila con ID 9 "FAILED"
-6.Hacer clic en el botón "FINALIZAR"</t>
-  </si>
-  <si>
     <t>Filtrar ont por estado en "FAILED"</t>
   </si>
   <si>
@@ -159,6 +151,15 @@
   </si>
   <si>
     <t>CP_GESTACT_003</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Seleccionar entidad"
+2.Seleccionar la fila que contiene el texto "elemento secundario
+3.Clic en botón "Siguiente"
+4.Seleccionar "ont"
+5.Clic en botón "Siguiente"
+6.Seleccionar fila con ID 9 "FAILED"
+7.Clic en botón "FINALIZAR"</t>
   </si>
 </sst>
 </file>
@@ -655,7 +656,7 @@
     </row>
     <row r="2" spans="1:13" ht="98.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>27</v>
@@ -694,10 +695,10 @@
     </row>
     <row r="3" spans="1:13" ht="148.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -709,7 +710,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>20</v>
@@ -733,10 +734,10 @@
     </row>
     <row r="4" spans="1:13" ht="124.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -748,16 +749,16 @@
         <v>19</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>16</v>

</xml_diff>